<commit_message>
Add Table 1 from Posthuma_2018 to use as topSS
</commit_message>
<xml_diff>
--- a/Data/GWAS/Posthuma_2018/Posthuma_2018_Table1.xlsx
+++ b/Data/GWAS/Posthuma_2018/Posthuma_2018_Table1.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Fine_Mapping/Data/GWAS/Posthuma_2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F097A000-79A9-794E-9318-A87351383890}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE153F44-E1F2-0A4A-9B91-D2D34EEFFB32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2360" windowWidth="27640" windowHeight="16940" xr2:uid="{CE451CDD-D4F5-C145-AFE6-E7326F9B9121}"/>
+    <workbookView xWindow="5580" yWindow="2360" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{CE451CDD-D4F5-C145-AFE6-E7326F9B9121}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="2" r:id="rId1"/>
     <sheet name="Table1_melted" sheetId="1" r:id="rId2"/>
+    <sheet name="Table1_melted_phase3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="208">
   <si>
     <t>Case-control status (phase 1)</t>
   </si>
@@ -4168,16 +4169,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4494,7 +4495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95EFEF8-F50F-F14B-9C14-5F111DE9D359}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -4507,27 +4508,27 @@
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="8" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -6089,7 +6090,7 @@
   <dimension ref="A1:L97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9783,4 +9784,1279 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDC03AA7-F3DA-AE4C-B438-91D034B0F126}">
+  <dimension ref="A1:L33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3">
+        <v>161155392</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="K2" s="3">
+        <v>6.36</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="3">
+        <v>207786828</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="K3" s="3">
+        <v>8.82</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="3">
+        <v>127891427</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="K4" s="3">
+        <v>13.94</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="3">
+        <v>233981912</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="3">
+        <v>57226150</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="K6" s="3">
+        <v>5.69</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="3">
+        <v>11026028</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.252</v>
+      </c>
+      <c r="K7" s="3">
+        <v>6</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="G8" s="3">
+        <v>11723235</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1.95</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="3">
+        <v>32583357</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.153</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="3">
+        <v>40942196</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="K10" s="3">
+        <v>8.26</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <v>6</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="3">
+        <v>47432637</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="K11" s="3">
+        <v>6.33</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="3">
+        <v>99971834</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
+        <v>7</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="3">
+        <v>143108158</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3">
+        <v>7</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="3">
+        <v>145950029</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K14" s="3">
+        <v>5.99</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="3">
+        <v>27464929</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3">
+        <v>10</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" s="3">
+        <v>11717397</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="K16" s="3">
+        <v>5.69</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3">
+        <v>11</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="3">
+        <v>59958380</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3">
+        <v>11</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G18" s="3">
+        <v>85776544</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.314</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3">
+        <v>11</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G19" s="3">
+        <v>121435587</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3">
+        <v>14</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G20" s="3">
+        <v>92938855</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3">
+        <v>15</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G21" s="3">
+        <v>59022615</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3">
+        <v>15</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G22" s="3">
+        <v>63569902</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="K22" s="3">
+        <v>5.52</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>21</v>
+      </c>
+      <c r="B23" s="3">
+        <v>16</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" s="3">
+        <v>31133100</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3">
+        <v>17</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G24" s="3">
+        <v>5138980</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="K24" s="3">
+        <v>6.12</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3">
+        <v>17</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G25" s="3">
+        <v>47450775</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="K25" s="3">
+        <v>5.62</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="3">
+        <v>17</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G26" s="3">
+        <v>56409089</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="3">
+        <v>18</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="G27" s="3">
+        <v>29088958</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>24</v>
+      </c>
+      <c r="B28" s="3">
+        <v>18</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G28" s="3">
+        <v>56189459</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J28" s="3">
+        <v>1.4E-2</v>
+      </c>
+      <c r="K28" s="3">
+        <v>5.52</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>25</v>
+      </c>
+      <c r="B29" s="3">
+        <v>19</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G29" s="3">
+        <v>1039323</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0.161</v>
+      </c>
+      <c r="K29" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>26</v>
+      </c>
+      <c r="B30" s="3">
+        <v>19</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G30" s="3">
+        <v>45351516</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J30" s="3">
+        <v>3.9E-2</v>
+      </c>
+      <c r="K30" s="3">
+        <v>35.5</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>27</v>
+      </c>
+      <c r="B31" s="3">
+        <v>19</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="G31" s="3">
+        <v>46241841</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J31" s="3">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="K31" s="3">
+        <v>5.46</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>28</v>
+      </c>
+      <c r="B32" s="3">
+        <v>19</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G32" s="3">
+        <v>51727962</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>29</v>
+      </c>
+      <c r="B33" s="3">
+        <v>20</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G33" s="3">
+        <v>54998544</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="3">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change p to e-10 notation
</commit_message>
<xml_diff>
--- a/Data/GWAS/Posthuma_2018/Posthuma_2018_Table1.xlsx
+++ b/Data/GWAS/Posthuma_2018/Posthuma_2018_Table1.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Fine_Mapping/Data/GWAS/Posthuma_2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE153F44-E1F2-0A4A-9B91-D2D34EEFFB32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4858B363-134C-ED4C-AE65-189462AFD9BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2360" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{CE451CDD-D4F5-C145-AFE6-E7326F9B9121}"/>
+    <workbookView xWindow="5580" yWindow="2260" windowWidth="29460" windowHeight="17040" activeTab="2" xr2:uid="{CE451CDD-D4F5-C145-AFE6-E7326F9B9121}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="2" r:id="rId1"/>
     <sheet name="Table1_melted" sheetId="1" r:id="rId2"/>
     <sheet name="Table1_melted_phase3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="239">
   <si>
     <t>Case-control status (phase 1)</t>
   </si>
@@ -4049,6 +4049,99 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>2.05E−10</t>
+  </si>
+  <si>
+    <t>1.10E−18</t>
+  </si>
+  <si>
+    <t>3.38E−44</t>
+  </si>
+  <si>
+    <t>8.92E−10</t>
+  </si>
+  <si>
+    <t>1.24E−8</t>
+  </si>
+  <si>
+    <t>1.93E−9</t>
+  </si>
+  <si>
+    <t>8.41E−11</t>
+  </si>
+  <si>
+    <t>1.45E−16</t>
+  </si>
+  <si>
+    <t>2.52E−10</t>
+  </si>
+  <si>
+    <t>2.22E−15</t>
+  </si>
+  <si>
+    <t>3.59E−11</t>
+  </si>
+  <si>
+    <t>2.10E−9</t>
+  </si>
+  <si>
+    <t>2.59E–4</t>
+  </si>
+  <si>
+    <t>2.61E−19</t>
+  </si>
+  <si>
+    <t>1.26E−8</t>
+  </si>
+  <si>
+    <t>1.55E−15</t>
+  </si>
+  <si>
+    <t>2.19E−18</t>
+  </si>
+  <si>
+    <t>1.09E−11</t>
+  </si>
+  <si>
+    <t>1.65E−10</t>
+  </si>
+  <si>
+    <t>1.31E−9</t>
+  </si>
+  <si>
+    <t>3.35E−8</t>
+  </si>
+  <si>
+    <t>3.98E−8</t>
+  </si>
+  <si>
+    <t>9.16E−10</t>
+  </si>
+  <si>
+    <t>1.87E−8</t>
+  </si>
+  <si>
+    <t>9.66E−7</t>
+  </si>
+  <si>
+    <t>3.30E−8</t>
+  </si>
+  <si>
+    <t>7.93E−11</t>
+  </si>
+  <si>
+    <t>5.79E−276</t>
+  </si>
+  <si>
+    <t>4.64E−8</t>
+  </si>
+  <si>
+    <t>6.34E−9</t>
+  </si>
+  <si>
+    <t>6.56E−10</t>
   </si>
 </sst>
 </file>
@@ -4162,7 +4255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4178,6 +4271,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9788,10 +9893,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDC03AA7-F3DA-AE4C-B438-91D034B0F126}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9800,6 +9905,8 @@
     <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="13" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -9818,7 +9925,7 @@
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -9840,7 +9947,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -9856,8 +9963,8 @@
       <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>20</v>
+      <c r="F2" s="11" t="s">
+        <v>208</v>
       </c>
       <c r="G2" s="3">
         <v>161155392</v>
@@ -9878,7 +9985,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -9894,8 +10001,8 @@
       <c r="E3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>28</v>
+      <c r="F3" s="11" t="s">
+        <v>209</v>
       </c>
       <c r="G3" s="3">
         <v>207786828</v>
@@ -9916,7 +10023,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -9932,8 +10039,8 @@
       <c r="E4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>35</v>
+      <c r="F4" s="11" t="s">
+        <v>210</v>
       </c>
       <c r="G4" s="3">
         <v>127891427</v>
@@ -9954,7 +10061,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -9970,8 +10077,8 @@
       <c r="E5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>41</v>
+      <c r="F5" s="11" t="s">
+        <v>211</v>
       </c>
       <c r="G5" s="3">
         <v>233981912</v>
@@ -9992,7 +10099,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -10008,8 +10115,8 @@
       <c r="E6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>46</v>
+      <c r="F6" s="11" t="s">
+        <v>212</v>
       </c>
       <c r="G6" s="3">
         <v>57226150</v>
@@ -10030,7 +10137,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -10046,8 +10153,8 @@
       <c r="E7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>53</v>
+      <c r="F7" s="11" t="s">
+        <v>213</v>
       </c>
       <c r="G7" s="3">
         <v>11026028</v>
@@ -10084,7 +10191,7 @@
       <c r="E8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="11">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="G8" s="3">
@@ -10106,7 +10213,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -10122,8 +10229,8 @@
       <c r="E9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>66</v>
+      <c r="F9" s="11" t="s">
+        <v>214</v>
       </c>
       <c r="G9" s="3">
         <v>32583357</v>
@@ -10144,7 +10251,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -10160,8 +10267,8 @@
       <c r="E10" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>69</v>
+      <c r="F10" s="11" t="s">
+        <v>215</v>
       </c>
       <c r="G10" s="3">
         <v>40942196</v>
@@ -10182,7 +10289,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -10198,8 +10305,8 @@
       <c r="E11" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>74</v>
+      <c r="F11" s="11" t="s">
+        <v>216</v>
       </c>
       <c r="G11" s="3">
         <v>47432637</v>
@@ -10220,7 +10327,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -10236,8 +10343,8 @@
       <c r="E12" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>81</v>
+      <c r="F12" s="11" t="s">
+        <v>217</v>
       </c>
       <c r="G12" s="3">
         <v>99971834</v>
@@ -10258,7 +10365,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -10274,8 +10381,8 @@
       <c r="E13" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>89</v>
+      <c r="F13" s="11" t="s">
+        <v>218</v>
       </c>
       <c r="G13" s="3">
         <v>143108158</v>
@@ -10312,8 +10419,8 @@
       <c r="E14" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>92</v>
+      <c r="F14" s="11" t="s">
+        <v>219</v>
       </c>
       <c r="G14" s="3">
         <v>145950029</v>
@@ -10325,7 +10432,7 @@
         <v>34</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>93</v>
+        <v>220</v>
       </c>
       <c r="K14" s="3">
         <v>5.99</v>
@@ -10334,7 +10441,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -10350,8 +10457,8 @@
       <c r="E15" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>100</v>
+      <c r="F15" s="11" t="s">
+        <v>221</v>
       </c>
       <c r="G15" s="3">
         <v>27464929</v>
@@ -10372,7 +10479,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -10388,8 +10495,8 @@
       <c r="E16" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>106</v>
+      <c r="F16" s="11" t="s">
+        <v>222</v>
       </c>
       <c r="G16" s="3">
         <v>11717397</v>
@@ -10410,7 +10517,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -10426,8 +10533,8 @@
       <c r="E17" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>114</v>
+      <c r="F17" s="11" t="s">
+        <v>223</v>
       </c>
       <c r="G17" s="3">
         <v>59958380</v>
@@ -10448,7 +10555,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -10464,8 +10571,8 @@
       <c r="E18" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>122</v>
+      <c r="F18" s="11" t="s">
+        <v>224</v>
       </c>
       <c r="G18" s="3">
         <v>85776544</v>
@@ -10486,7 +10593,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -10502,8 +10609,8 @@
       <c r="E19" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>128</v>
+      <c r="F19" s="11" t="s">
+        <v>225</v>
       </c>
       <c r="G19" s="3">
         <v>121435587</v>
@@ -10524,7 +10631,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -10540,8 +10647,8 @@
       <c r="E20" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>134</v>
+      <c r="F20" s="11" t="s">
+        <v>226</v>
       </c>
       <c r="G20" s="3">
         <v>92938855</v>
@@ -10562,7 +10669,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -10578,8 +10685,8 @@
       <c r="E21" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>140</v>
+      <c r="F21" s="11" t="s">
+        <v>227</v>
       </c>
       <c r="G21" s="3">
         <v>59022615</v>
@@ -10600,7 +10707,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -10616,8 +10723,8 @@
       <c r="E22" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>144</v>
+      <c r="F22" s="11" t="s">
+        <v>228</v>
       </c>
       <c r="G22" s="3">
         <v>63569902</v>
@@ -10638,7 +10745,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -10654,8 +10761,8 @@
       <c r="E23" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>150</v>
+      <c r="F23" s="11" t="s">
+        <v>229</v>
       </c>
       <c r="G23" s="3">
         <v>31133100</v>
@@ -10676,7 +10783,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -10692,8 +10799,8 @@
       <c r="E24" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>156</v>
+      <c r="F24" s="11" t="s">
+        <v>230</v>
       </c>
       <c r="G24" s="3">
         <v>5138980</v>
@@ -10714,7 +10821,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -10730,8 +10837,8 @@
       <c r="E25" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>161</v>
+      <c r="F25" s="11" t="s">
+        <v>231</v>
       </c>
       <c r="G25" s="3">
         <v>47450775</v>
@@ -10768,8 +10875,8 @@
       <c r="E26" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>166</v>
+      <c r="F26" s="11" t="s">
+        <v>232</v>
       </c>
       <c r="G26" s="3">
         <v>56409089</v>
@@ -10806,7 +10913,7 @@
       <c r="E27" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="11">
         <v>0.03</v>
       </c>
       <c r="G27" s="3">
@@ -10828,7 +10935,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>24</v>
       </c>
@@ -10844,8 +10951,8 @@
       <c r="E28" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>175</v>
+      <c r="F28" s="11" t="s">
+        <v>233</v>
       </c>
       <c r="G28" s="3">
         <v>56189459</v>
@@ -10866,7 +10973,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>25</v>
       </c>
@@ -10882,8 +10989,8 @@
       <c r="E29" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>182</v>
+      <c r="F29" s="11" t="s">
+        <v>234</v>
       </c>
       <c r="G29" s="3">
         <v>1039323</v>
@@ -10904,7 +11011,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>26</v>
       </c>
@@ -10920,8 +11027,8 @@
       <c r="E30" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>188</v>
+      <c r="F30" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="G30" s="3">
         <v>45351516</v>
@@ -10942,7 +11049,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>27</v>
       </c>
@@ -10958,8 +11065,8 @@
       <c r="E31" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="F31" s="4" t="s">
-        <v>193</v>
+      <c r="F31" s="11" t="s">
+        <v>236</v>
       </c>
       <c r="G31" s="3">
         <v>46241841</v>
@@ -10980,7 +11087,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>28</v>
       </c>
@@ -10996,8 +11103,8 @@
       <c r="E32" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>200</v>
+      <c r="F32" s="11" t="s">
+        <v>237</v>
       </c>
       <c r="G32" s="3">
         <v>51727962</v>
@@ -11018,7 +11125,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>29</v>
       </c>
@@ -11034,8 +11141,8 @@
       <c r="E33" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="F33" s="4" t="s">
-        <v>206</v>
+      <c r="F33" s="11" t="s">
+        <v>238</v>
       </c>
       <c r="G33" s="3">
         <v>54998544</v>
@@ -11055,6 +11162,9 @@
       <c r="L33" s="3" t="s">
         <v>42</v>
       </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F35" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tinkering with plot zooms
</commit_message>
<xml_diff>
--- a/Data/GWAS/Posthuma_2018/Posthuma_2018_Table1.xlsx
+++ b/Data/GWAS/Posthuma_2018/Posthuma_2018_Table1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Fine_Mapping/Data/GWAS/Posthuma_2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD614FF7-BC59-304B-B25F-4AAF7CE996EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929279B1-6892-654D-8FD8-AF258C9210E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="2260" windowWidth="29460" windowHeight="17040" activeTab="2" xr2:uid="{CE451CDD-D4F5-C145-AFE6-E7326F9B9121}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="240">
   <si>
     <t>Case-control status (phase 1)</t>
   </si>
@@ -4142,6 +4142,9 @@
   </si>
   <si>
     <t>6.56E−10</t>
+  </si>
+  <si>
+    <t>P_exp</t>
   </si>
 </sst>
 </file>
@@ -4263,15 +4266,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4283,6 +4277,15 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4616,24 +4619,24 @@
     <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="7" t="s">
+      <c r="G1" s="12"/>
+      <c r="H1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -6194,8 +6197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54EB7753-104A-0C4B-91C1-BB092A23701C}">
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="F97" sqref="F66:F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9893,10 +9896,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDC03AA7-F3DA-AE4C-B438-91D034B0F126}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9905,11 +9908,12 @@
     <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="12" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" customWidth="1"/>
+    <col min="7" max="7" width="22" style="9" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -9925,29 +9929,32 @@
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -9963,29 +9970,32 @@
       <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>161155392</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="3">
         <v>0.24</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="3">
         <v>6.36</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -10001,29 +10011,32 @@
       <c r="E3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>207786828</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="3">
+      <c r="K3" s="3">
         <v>0.20499999999999999</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>8.82</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -10039,29 +10052,32 @@
       <c r="E4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>127891427</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>0.41499999999999998</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>13.94</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -10077,29 +10093,32 @@
       <c r="E5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>233981912</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <v>0.23499999999999999</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -10115,29 +10134,32 @@
       <c r="E6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>57226150</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="3">
+      <c r="K6" s="3">
         <v>2E-3</v>
       </c>
-      <c r="K6" s="3">
+      <c r="L6" s="3">
         <v>5.69</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -10153,29 +10175,32 @@
       <c r="E7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>11026028</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="3">
+      <c r="K7" s="3">
         <v>0.252</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L7" s="3">
         <v>6</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>55</v>
       </c>
@@ -10191,29 +10216,32 @@
       <c r="E8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="3">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="10">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="H8" s="3">
         <v>11723235</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="3">
+      <c r="K8" s="3">
         <v>0.29099999999999998</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L8" s="3">
         <v>1.95</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -10229,29 +10257,32 @@
       <c r="E9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>32583357</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="3">
+      <c r="K9" s="3">
         <v>0.153</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -10267,29 +10298,32 @@
       <c r="E10" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>40942196</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="3">
+      <c r="K10" s="3">
         <v>2E-3</v>
       </c>
-      <c r="K10" s="3">
+      <c r="L10" s="3">
         <v>8.26</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -10305,29 +10339,32 @@
       <c r="E11" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>47432637</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J11" s="3">
+      <c r="K11" s="3">
         <v>0.35499999999999998</v>
       </c>
-      <c r="K11" s="3">
+      <c r="L11" s="3">
         <v>6.33</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -10343,29 +10380,32 @@
       <c r="E12" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="3">
         <v>99971834</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="J12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="3">
+      <c r="K12" s="3">
         <v>0.31</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="L12" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="M12" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -10381,29 +10421,32 @@
       <c r="E13" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H13" s="3">
         <v>143108158</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="3">
+      <c r="K13" s="3">
         <v>0.5</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="L13" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="M13" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -10419,29 +10462,32 @@
       <c r="E14" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="G14" s="3">
+      <c r="H14" s="3">
         <v>145950029</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="J14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="K14" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L14" s="3">
         <v>5.99</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="M14" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -10457,29 +10503,32 @@
       <c r="E15" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="G15" s="3">
+      <c r="H15" s="3">
         <v>27464929</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="J15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="3">
+      <c r="K15" s="3">
         <v>0.39100000000000001</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="L15" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="M15" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -10495,29 +10544,32 @@
       <c r="E16" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="G16" s="3">
+      <c r="H16" s="3">
         <v>11717397</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="3">
+      <c r="K16" s="3">
         <v>0.375</v>
       </c>
-      <c r="K16" s="3">
+      <c r="L16" s="3">
         <v>5.69</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -10533,29 +10585,32 @@
       <c r="E17" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="G17" s="3">
+      <c r="H17" s="3">
         <v>59958380</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="J17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="3">
+      <c r="K17" s="3">
         <v>0.38100000000000001</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="L17" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="M17" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -10571,29 +10626,32 @@
       <c r="E18" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G18" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="G18" s="3">
+      <c r="H18" s="3">
         <v>85776544</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="J18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="3">
+      <c r="K18" s="3">
         <v>0.314</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="M18" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -10609,29 +10667,32 @@
       <c r="E19" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G19" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="G19" s="3">
+      <c r="H19" s="3">
         <v>121435587</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="I19" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="J19" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="3">
+      <c r="K19" s="3">
         <v>0.04</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="L19" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="M19" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -10647,29 +10708,32 @@
       <c r="E20" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G20" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="G20" s="3">
+      <c r="H20" s="3">
         <v>92938855</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="I20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="J20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="3">
+      <c r="K20" s="3">
         <v>0.34399999999999997</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="L20" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="M20" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -10685,29 +10749,32 @@
       <c r="E21" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="G21" s="3">
+      <c r="H21" s="3">
         <v>59022615</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="I21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="J21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="3">
+      <c r="K21" s="3">
         <v>0.32</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="L21" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="M21" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -10723,29 +10790,32 @@
       <c r="E22" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G22" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="G22" s="3">
+      <c r="H22" s="3">
         <v>63569902</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J22" s="3">
+      <c r="K22" s="3">
         <v>0.13200000000000001</v>
       </c>
-      <c r="K22" s="3">
+      <c r="L22" s="3">
         <v>5.52</v>
       </c>
-      <c r="L22" s="3" t="s">
+      <c r="M22" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -10761,29 +10831,32 @@
       <c r="E23" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="G23" s="3">
+      <c r="H23" s="3">
         <v>31133100</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J23" s="3">
+      <c r="K23" s="3">
         <v>0.3</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="L23" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="M23" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -10799,29 +10872,32 @@
       <c r="E24" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="G24" s="3">
+      <c r="H24" s="3">
         <v>5138980</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="J24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J24" s="3">
+      <c r="K24" s="3">
         <v>0.12</v>
       </c>
-      <c r="K24" s="3">
+      <c r="L24" s="3">
         <v>6.12</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="M24" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -10837,29 +10913,32 @@
       <c r="E25" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F25" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G25" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="G25" s="3">
+      <c r="H25" s="3">
         <v>47450775</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="J25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J25" s="3">
+      <c r="K25" s="3">
         <v>0.47299999999999998</v>
       </c>
-      <c r="K25" s="3">
+      <c r="L25" s="3">
         <v>5.62</v>
       </c>
-      <c r="L25" s="3" t="s">
+      <c r="M25" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="19" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>55</v>
       </c>
@@ -10875,29 +10954,32 @@
       <c r="E26" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="F26" s="13" t="s">
+      <c r="F26" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G26" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="G26" s="3">
+      <c r="H26" s="3">
         <v>56409089</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="J26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="3">
+      <c r="K26" s="3">
         <v>0.45500000000000002</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="L26" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="M26" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>55</v>
       </c>
@@ -10913,29 +10995,32 @@
       <c r="E27" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27" s="3">
         <v>0.03</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="H27" s="3">
         <v>29088958</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="I27" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="J27" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J27" s="3">
+      <c r="K27" s="3">
         <v>0.01</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="L27" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="L27" s="3" t="s">
+      <c r="M27" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>24</v>
       </c>
@@ -10951,29 +11036,32 @@
       <c r="E28" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G28" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="G28" s="3">
+      <c r="H28" s="3">
         <v>56189459</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="I28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="J28" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J28" s="3">
+      <c r="K28" s="3">
         <v>1.4E-2</v>
       </c>
-      <c r="K28" s="3">
+      <c r="L28" s="3">
         <v>5.52</v>
       </c>
-      <c r="L28" s="3" t="s">
+      <c r="M28" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>25</v>
       </c>
@@ -10989,29 +11077,32 @@
       <c r="E29" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="F29" s="13" t="s">
+      <c r="F29" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G29" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="G29" s="3">
+      <c r="H29" s="3">
         <v>1039323</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="I29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="J29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J29" s="3">
+      <c r="K29" s="3">
         <v>0.161</v>
       </c>
-      <c r="K29" s="3">
+      <c r="L29" s="3">
         <v>6.5</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="M29" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>26</v>
       </c>
@@ -11027,29 +11118,32 @@
       <c r="E30" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F30" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G30" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="G30" s="3">
+      <c r="H30" s="3">
         <v>45351516</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="I30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="J30" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J30" s="3">
+      <c r="K30" s="3">
         <v>3.9E-2</v>
       </c>
-      <c r="K30" s="3">
+      <c r="L30" s="3">
         <v>35.5</v>
       </c>
-      <c r="L30" s="3" t="s">
+      <c r="M30" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>27</v>
       </c>
@@ -11065,29 +11159,32 @@
       <c r="E31" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="G31" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="G31" s="3">
+      <c r="H31" s="3">
         <v>46241841</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="I31" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="J31" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J31" s="3">
+      <c r="K31" s="3">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="K31" s="3">
+      <c r="L31" s="3">
         <v>5.46</v>
       </c>
-      <c r="L31" s="3" t="s">
+      <c r="M31" s="3" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>28</v>
       </c>
@@ -11103,29 +11200,32 @@
       <c r="E32" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F32" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G32" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="G32" s="3">
+      <c r="H32" s="3">
         <v>51727962</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="I32" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I32" s="3" t="s">
+      <c r="J32" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J32" s="3">
+      <c r="K32" s="3">
         <v>0.32</v>
       </c>
-      <c r="K32" s="3" t="s">
+      <c r="L32" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="L32" s="3" t="s">
+      <c r="M32" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>29</v>
       </c>
@@ -11141,30 +11241,33 @@
       <c r="E33" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="F33" s="13" t="s">
+      <c r="F33" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G33" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="G33" s="3">
+      <c r="H33" s="3">
         <v>54998544</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="I33" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="J33" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="3">
+      <c r="K33" s="3">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="L33" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="L33" s="3" t="s">
+      <c r="M33" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F35" s="11"/>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G35" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>